<commit_message>
Further animating 5 year change
</commit_message>
<xml_diff>
--- a/Research/Using 5 year bands for aging/5YearChange.xlsx
+++ b/Research/Using 5 year bands for aging/5YearChange.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\HepatitisCModel\Research\Using 5 year bands for aging\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="15480" windowHeight="7020"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="15480" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +19,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Starting year</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Expected</t>
   </si>
 </sst>
 </file>
@@ -79,6 +92,679 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Starting year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.960000000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.960000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Year 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.768000000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.960000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.480000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2000000000000008E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="162555392"/>
+        <c:axId val="218927616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="162555392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="218927616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="218927616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="162555392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,7 +1022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -344,35 +1030,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G11"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15</v>
       </c>
@@ -399,8 +1088,11 @@
         <f t="shared" ref="G2" si="1">F2*0.8</f>
         <v>0</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+5</f>
         <v>20</v>
@@ -428,8 +1120,12 @@
         <f t="shared" ref="G3" si="3">F3*0.8+0.2*F2</f>
         <v>32.768000000000008</v>
       </c>
+      <c r="H3">
+        <f>B2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="4">A3+5</f>
         <v>25</v>
@@ -457,8 +1153,12 @@
         <f t="shared" ref="G4" si="6">F4*0.8+0.2*F3</f>
         <v>40.960000000000008</v>
       </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="7">B3</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="4"/>
         <v>30</v>
@@ -483,11 +1183,15 @@
         <v>15.360000000000003</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5" si="7">F5*0.8+0.2*F4</f>
+        <f t="shared" ref="G5" si="8">F5*0.8+0.2*F4</f>
         <v>20.480000000000004</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="4"/>
         <v>35</v>
@@ -512,11 +1216,15 @@
         <v>2.5600000000000005</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6" si="8">F6*0.8+0.2*F5</f>
+        <f t="shared" ref="G6" si="9">F6*0.8+0.2*F5</f>
         <v>5.120000000000001</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="4"/>
         <v>40</v>
@@ -541,11 +1249,15 @@
         <v>0.16000000000000003</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7" si="9">F7*0.8+0.2*F6</f>
+        <f t="shared" ref="G7" si="10">F7*0.8+0.2*F6</f>
         <v>0.64000000000000012</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="4"/>
         <v>45</v>
@@ -570,98 +1282,19 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8" si="10">F8*0.8+0.2*F7</f>
+        <f t="shared" ref="G8" si="11">F8*0.8+0.2*F7</f>
         <v>3.2000000000000008E-2</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ref="G9" si="11">F9*0.8+0.2*F8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="4"/>
-        <v>55</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ref="G10" si="12">F10*0.8+0.2*F9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="shared" ref="G11" si="13">F11*0.8+0.2*F10</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>